<commit_message>
CHE pop for 2020 # 78
</commit_message>
<xml_diff>
--- a/data-raw/BfS/su-e-01.02.04.05.xlsx
+++ b/data-raw/BfS/su-e-01.02.04.05.xlsx
@@ -5,20 +5,20 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\SKS\DIAM\30_Input\Diffusion\01\2020-0182_27.08.2020\Tabellen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\KOM_PUB\DIAM\30_Input\DEM\GNP 2021-0180_01.09.2021\Tabellen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="-12" windowWidth="25260" windowHeight="5256"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="25260" windowHeight="5250"/>
   </bookViews>
   <sheets>
     <sheet name="su-e-01.02.04.05" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'su-e-01.02.04.05'!$A$1:$N$181</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'su-e-01.02.04.05'!$A$1:$N$179</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'su-e-01.02.04.05'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcMode="manual"/>
 </workbook>
 </file>
 
@@ -332,7 +332,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>, 1861-2019</t>
+      <t>, 1861-2020</t>
     </r>
   </si>
 </sst>
@@ -569,7 +569,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="167" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -679,6 +679,9 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="167" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -1067,7 +1070,7 @@
   <sheetPr codeName="Feuil1">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:M179"/>
+  <dimension ref="A1:M180"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
@@ -1076,18 +1079,18 @@
       <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" style="14" customWidth="1"/>
-    <col min="3" max="6" width="11.6640625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" style="14" customWidth="1"/>
+    <col min="3" max="6" width="11.7265625" style="14" customWidth="1"/>
     <col min="7" max="7" width="12" style="14" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" style="14" customWidth="1"/>
-    <col min="9" max="10" width="11.6640625" style="14" customWidth="1"/>
-    <col min="11" max="11" width="12.88671875" style="14" customWidth="1"/>
-    <col min="12" max="12" width="10.88671875" style="14" customWidth="1"/>
-    <col min="13" max="13" width="8.33203125" style="14" customWidth="1"/>
-    <col min="14" max="16384" width="11.44140625" style="14"/>
+    <col min="8" max="8" width="12.453125" style="14" customWidth="1"/>
+    <col min="9" max="10" width="11.7265625" style="14" customWidth="1"/>
+    <col min="11" max="11" width="12.81640625" style="14" customWidth="1"/>
+    <col min="12" max="12" width="10.81640625" style="14" customWidth="1"/>
+    <col min="13" max="13" width="8.26953125" style="14" customWidth="1"/>
+    <col min="14" max="16384" width="11.453125" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="4" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -1099,9 +1102,9 @@
       </c>
       <c r="K1" s="5"/>
     </row>
-    <row r="2" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -1122,7 +1125,7 @@
       </c>
       <c r="M2" s="13"/>
     </row>
-    <row r="3" spans="1:13" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" s="20" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15"/>
       <c r="B3" s="7" t="s">
         <v>17</v>
@@ -1145,7 +1148,7 @@
       <c r="H3" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="43" t="s">
+      <c r="I3" s="44" t="s">
         <v>32</v>
       </c>
       <c r="J3" s="16" t="s">
@@ -1161,8 +1164,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" s="20" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15"/>
+      <c r="B4" s="43"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7" t="s">
@@ -1171,7 +1175,7 @@
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
-      <c r="I4" s="44"/>
+      <c r="I4" s="45"/>
       <c r="J4" s="7" t="s">
         <v>2</v>
       </c>
@@ -1181,7 +1185,7 @@
       </c>
       <c r="M4" s="21"/>
     </row>
-    <row r="5" spans="1:13" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" s="20" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="23"/>
       <c r="B5" s="24"/>
       <c r="C5" s="25"/>
@@ -1190,7 +1194,7 @@
       <c r="F5" s="25"/>
       <c r="G5" s="25"/>
       <c r="H5" s="25"/>
-      <c r="I5" s="45"/>
+      <c r="I5" s="46"/>
       <c r="J5" s="26"/>
       <c r="K5" s="27"/>
       <c r="L5" s="28"/>
@@ -1237,7 +1241,7 @@
         <v>0.70291119171693051</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="30">
         <v>1862</v>
       </c>
@@ -1278,7 +1282,7 @@
         <v>0.83613723546500951</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="30">
         <v>1863</v>
       </c>
@@ -1319,7 +1323,7 @@
         <v>0.83750382205079599</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="30">
         <v>1864</v>
       </c>
@@ -1360,7 +1364,7 @@
         <v>0.73402858852273734</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="30">
         <v>1865</v>
       </c>
@@ -1401,7 +1405,7 @@
         <v>0.63775869079668768</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="30">
         <v>1866</v>
       </c>
@@ -1442,7 +1446,7 @@
         <v>0.54758488944514616</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="30">
         <v>1867</v>
       </c>
@@ -1483,7 +1487,7 @@
         <v>0.4623295497828902</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="30">
         <v>1868</v>
       </c>
@@ -1524,7 +1528,7 @@
         <v>0.38084759347543051</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="30">
         <v>1869</v>
       </c>
@@ -1606,7 +1610,7 @@
         <v>0.59655013858295447</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="30">
         <v>1871</v>
       </c>
@@ -1647,7 +1651,7 @@
         <v>0.49187048432971703</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="30">
         <v>1872</v>
       </c>
@@ -1688,7 +1692,7 @@
         <v>0.5718714011444872</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="30">
         <v>1873</v>
       </c>
@@ -1729,7 +1733,7 @@
         <v>0.59682114832741306</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="30">
         <v>1874</v>
       </c>
@@ -1770,7 +1774,7 @@
         <v>0.56579797417909805</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="30">
         <v>1875</v>
       </c>
@@ -1811,7 +1815,7 @@
         <v>0.58189411546497205</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="30">
         <v>1876</v>
       </c>
@@ -1852,7 +1856,7 @@
         <v>0.66461942690622988</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="30">
         <v>1877</v>
       </c>
@@ -1893,7 +1897,7 @@
         <v>0.64487550159592955</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="30">
         <v>1878</v>
       </c>
@@ -1934,7 +1938,7 @@
         <v>0.59981748431348758</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="30">
         <v>1879</v>
       </c>
@@ -2016,7 +2020,7 @@
         <v>0.82326846169054357</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="30">
         <v>1881</v>
       </c>
@@ -2057,7 +2061,7 @@
         <v>0.37859518444105461</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="30">
         <v>1882</v>
       </c>
@@ -2098,7 +2102,7 @@
         <v>0.31491395894088742</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="30">
         <v>1883</v>
       </c>
@@ -2139,7 +2143,7 @@
         <v>0.38563278389110822</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="30">
         <v>1884</v>
       </c>
@@ -2180,7 +2184,7 @@
         <v>0.43207451491747184</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="30">
         <v>1885</v>
       </c>
@@ -2221,7 +2225,7 @@
         <v>0.29524876286121504</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="30">
         <v>1886</v>
       </c>
@@ -2262,7 +2266,7 @@
         <v>0.32573999441252699</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="30">
         <v>1887</v>
       </c>
@@ -2303,7 +2307,7 @@
         <v>0.33181635680942101</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="30">
         <v>1888</v>
       </c>
@@ -2344,7 +2348,7 @@
         <v>0.40065498020941642</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="30">
         <v>1889</v>
       </c>
@@ -2426,7 +2430,7 @@
         <v>0.76102437739377538</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="30">
         <v>1891</v>
       </c>
@@ -2467,7 +2471,7 @@
         <v>0.96257634527850378</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="30">
         <v>1892</v>
       </c>
@@ -2508,7 +2512,7 @@
         <v>1.0768731387254418</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="30">
         <v>1893</v>
       </c>
@@ -2549,7 +2553,7 @@
         <v>0.99813877271101181</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="30">
         <v>1894</v>
       </c>
@@ -2590,7 +2594,7 @@
         <v>0.92605227574400517</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="30">
         <v>1895</v>
       </c>
@@ -2631,7 +2635,7 @@
         <v>1.0028512882550535</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="30">
         <v>1896</v>
       </c>
@@ -2672,7 +2676,7 @@
         <v>1.2387797433475876</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="30">
         <v>1897</v>
       </c>
@@ -2713,7 +2717,7 @@
         <v>1.2661679432101836</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="30">
         <v>1898</v>
       </c>
@@ -2754,7 +2758,7 @@
         <v>1.2384039224089729</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="30">
         <v>1899</v>
       </c>
@@ -2836,7 +2840,7 @@
         <v>1.1143651594698647</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="30">
         <v>1901</v>
       </c>
@@ -2877,7 +2881,7 @@
         <v>1.3584876099168872</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="30">
         <v>1902</v>
       </c>
@@ -2918,7 +2922,7 @@
         <v>1.3989589405461773</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="30">
         <v>1903</v>
       </c>
@@ -2959,7 +2963,7 @@
         <v>1.2482941894706601</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="30">
         <v>1904</v>
       </c>
@@ -3000,7 +3004,7 @@
         <v>1.22974790052222</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="30">
         <v>1905</v>
       </c>
@@ -3041,7 +3045,7 @@
         <v>1.1626091045447213</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="30">
         <v>1906</v>
       </c>
@@ -3082,7 +3086,7 @@
         <v>1.2812585263378133</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="30">
         <v>1907</v>
       </c>
@@ -3123,7 +3127,7 @@
         <v>1.2089105121475894</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="30">
         <v>1908</v>
       </c>
@@ -3164,7 +3168,7 @@
         <v>1.2607793336893345</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="30">
         <v>1909</v>
       </c>
@@ -3246,7 +3250,7 @@
         <v>1.2116271376029535</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="30">
         <v>1911</v>
       </c>
@@ -3287,7 +3291,7 @@
         <v>0.57149062962988595</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="30">
         <v>1912</v>
       </c>
@@ -3328,7 +3332,7 @@
         <v>0.7220949461029158</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="30">
         <v>1913</v>
       </c>
@@ -3369,7 +3373,7 @@
         <v>0.6000638533527608</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="30">
         <v>1914</v>
       </c>
@@ -3410,7 +3414,7 @@
         <v>0.55727790314099956</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="30">
         <v>1915</v>
       </c>
@@ -3451,7 +3455,7 @@
         <v>0.2823288480390756</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="30">
         <v>1916</v>
       </c>
@@ -3492,7 +3496,7 @@
         <v>0.28816502984612635</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="30">
         <v>1917</v>
       </c>
@@ -3533,7 +3537,7 @@
         <v>0.1843089447693039</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="30">
         <v>1918</v>
       </c>
@@ -3574,7 +3578,7 @@
         <v>-0.36226802677875353</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="30">
         <v>1919</v>
       </c>
@@ -3656,7 +3660,7 @@
         <v>0.35867859281386832</v>
       </c>
     </row>
-    <row r="66" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="30">
         <v>1921</v>
       </c>
@@ -3697,7 +3701,7 @@
         <v>0.6479182975567549</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="30">
         <v>1922</v>
       </c>
@@ -3738,7 +3742,7 @@
         <v>0.51285383908644733</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="30">
         <v>1923</v>
       </c>
@@ -3779,7 +3783,7 @@
         <v>0.59991355624418685</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="30">
         <v>1924</v>
       </c>
@@ -3820,7 +3824,7 @@
         <v>0.46931607076075865</v>
       </c>
     </row>
-    <row r="70" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="30">
         <v>1925</v>
       </c>
@@ -3861,7 +3865,7 @@
         <v>0.46704823000179818</v>
       </c>
     </row>
-    <row r="71" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="30">
         <v>1926</v>
       </c>
@@ -3902,7 +3906,7 @@
         <v>0.50912119064670924</v>
       </c>
     </row>
-    <row r="72" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="30">
         <v>1927</v>
       </c>
@@ -3943,7 +3947,7 @@
         <v>0.36931945010109646</v>
       </c>
     </row>
-    <row r="73" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="30">
         <v>1928</v>
       </c>
@@ -3984,7 +3988,7 @@
         <v>0.39340563495425962</v>
       </c>
     </row>
-    <row r="74" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="30">
         <v>1929</v>
       </c>
@@ -4066,7 +4070,7 @@
         <v>0.43145599185896705</v>
       </c>
     </row>
-    <row r="76" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="30">
         <v>1931</v>
       </c>
@@ -4107,7 +4111,7 @@
         <v>0.52972426328770073</v>
       </c>
     </row>
-    <row r="77" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="30">
         <v>1932</v>
       </c>
@@ -4148,7 +4152,7 @@
         <v>0.45913556597147032</v>
       </c>
     </row>
-    <row r="78" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="30">
         <v>1933</v>
       </c>
@@ -4189,7 +4193,7 @@
         <v>0.63144890458029757</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="30">
         <v>1934</v>
       </c>
@@ -4230,7 +4234,7 @@
         <v>0.56462919056761007</v>
       </c>
     </row>
-    <row r="80" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="30">
         <v>1935</v>
       </c>
@@ -4271,7 +4275,7 @@
         <v>0.45536959654282599</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="30">
         <v>1936</v>
       </c>
@@ -4312,7 +4316,7 @@
         <v>0.48202285911205561</v>
       </c>
     </row>
-    <row r="82" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="30">
         <v>1937</v>
       </c>
@@ -4353,7 +4357,7 @@
         <v>0.4368886024566172</v>
       </c>
     </row>
-    <row r="83" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="30">
         <v>1938</v>
       </c>
@@ -4394,7 +4398,7 @@
         <v>0.43403967536184601</v>
       </c>
     </row>
-    <row r="84" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="30">
         <v>1939</v>
       </c>
@@ -4476,7 +4480,7 @@
         <v>0.37767152875848065</v>
       </c>
     </row>
-    <row r="86" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="30">
         <v>1941</v>
       </c>
@@ -4517,7 +4521,7 @@
         <v>0.64954869612393074</v>
       </c>
     </row>
-    <row r="87" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="30">
         <v>1942</v>
       </c>
@@ -4558,7 +4562,7 @@
         <v>0.70009656263549669</v>
       </c>
     </row>
-    <row r="88" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="30">
         <v>1943</v>
       </c>
@@ -4599,7 +4603,7 @@
         <v>0.78365544398667464</v>
       </c>
     </row>
-    <row r="89" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="30">
         <v>1944</v>
       </c>
@@ -4640,7 +4644,7 @@
         <v>0.72552887954885947</v>
       </c>
     </row>
-    <row r="90" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="30">
         <v>1945</v>
       </c>
@@ -4681,7 +4685,7 @@
         <v>0.81501366362506911</v>
       </c>
     </row>
-    <row r="91" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="30">
         <v>1946</v>
       </c>
@@ -4722,7 +4726,7 @@
         <v>1.3975014661988381</v>
       </c>
     </row>
-    <row r="92" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="30">
         <v>1947</v>
       </c>
@@ -4763,7 +4767,7 @@
         <v>1.3162583518930957</v>
       </c>
     </row>
-    <row r="93" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="30">
         <v>1948</v>
       </c>
@@ -4804,7 +4808,7 @@
         <v>1.3651051856411158</v>
       </c>
     </row>
-    <row r="94" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="30">
         <v>1949</v>
       </c>
@@ -4886,7 +4890,7 @@
         <v>1.0539845758354756</v>
       </c>
     </row>
-    <row r="96" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="30">
         <v>1951</v>
       </c>
@@ -4927,7 +4931,7 @@
         <v>1.3079793097600272</v>
       </c>
     </row>
-    <row r="97" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="30">
         <v>1952</v>
       </c>
@@ -4968,7 +4972,7 @@
         <v>1.3643307037184289</v>
       </c>
     </row>
-    <row r="98" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="30">
         <v>1953</v>
       </c>
@@ -5009,7 +5013,7 @@
         <v>1.2984868190169485</v>
       </c>
     </row>
-    <row r="99" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="30">
         <v>1954</v>
       </c>
@@ -5050,7 +5054,7 @@
         <v>1.2899938862848992</v>
       </c>
     </row>
-    <row r="100" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="30">
         <v>1955</v>
       </c>
@@ -5091,7 +5095,7 @@
         <v>1.2755769269460597</v>
       </c>
     </row>
-    <row r="101" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="30">
         <v>1956</v>
       </c>
@@ -5132,7 +5136,7 @@
         <v>1.2654707272980115</v>
       </c>
     </row>
-    <row r="102" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="30">
         <v>1957</v>
       </c>
@@ -5173,7 +5177,7 @@
         <v>1.2830070231882922</v>
       </c>
     </row>
-    <row r="103" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="30">
         <v>1958</v>
       </c>
@@ -5214,7 +5218,7 @@
         <v>1.3016192763616641</v>
       </c>
     </row>
-    <row r="104" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="30">
         <v>1959</v>
       </c>
@@ -5296,7 +5300,7 @@
         <v>1.2209045415919175</v>
       </c>
     </row>
-    <row r="106" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="30">
         <v>1961</v>
       </c>
@@ -5337,7 +5341,7 @@
         <v>2.7663762582896418</v>
       </c>
     </row>
-    <row r="107" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="30">
         <v>1962</v>
       </c>
@@ -5378,7 +5382,7 @@
         <v>2.3738139780173495</v>
       </c>
     </row>
-    <row r="108" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="30">
         <v>1963</v>
       </c>
@@ -5419,7 +5423,7 @@
         <v>1.9524772596088626</v>
       </c>
     </row>
-    <row r="109" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="30">
         <v>1964</v>
       </c>
@@ -5460,7 +5464,7 @@
         <v>1.3889867269035756</v>
       </c>
     </row>
-    <row r="110" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="30">
         <v>1965</v>
       </c>
@@ -5501,7 +5505,7 @@
         <v>0.93721972786454855</v>
       </c>
     </row>
-    <row r="111" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="30">
         <v>1966</v>
       </c>
@@ -5542,7 +5546,7 @@
         <v>1.1629922764042484</v>
       </c>
     </row>
-    <row r="112" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="30">
         <v>1967</v>
       </c>
@@ -5583,7 +5587,7 @@
         <v>1.329538444169365</v>
       </c>
     </row>
-    <row r="113" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="30">
         <v>1968</v>
       </c>
@@ -5624,7 +5628,7 @@
         <v>1.2057161966809105</v>
       </c>
     </row>
-    <row r="114" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="30">
         <v>1969</v>
       </c>
@@ -5706,7 +5710,7 @@
         <v>0.39496166129006111</v>
       </c>
     </row>
-    <row r="116" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="30">
         <v>1971</v>
       </c>
@@ -5747,7 +5751,7 @@
         <v>0.65686387222867393</v>
       </c>
     </row>
-    <row r="117" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="30">
         <v>1972</v>
       </c>
@@ -5788,7 +5792,7 @@
         <v>0.87305478056205055</v>
       </c>
     </row>
-    <row r="118" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="30">
         <v>1973</v>
       </c>
@@ -5829,7 +5833,7 @@
         <v>0.60998688330210005</v>
       </c>
     </row>
-    <row r="119" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="30">
         <v>1974</v>
       </c>
@@ -5870,7 +5874,7 @@
         <v>0.47040041729069276</v>
       </c>
     </row>
-    <row r="120" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="30">
         <v>1975</v>
       </c>
@@ -5911,7 +5915,7 @@
         <v>-0.55546596793567315</v>
       </c>
     </row>
-    <row r="121" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="30">
         <v>1976</v>
       </c>
@@ -5952,7 +5956,7 @@
         <v>-0.58454561936459837</v>
       </c>
     </row>
-    <row r="122" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="30">
         <v>1977</v>
       </c>
@@ -5993,7 +5997,7 @@
         <v>-9.0865271309218967E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="30">
         <v>1978</v>
       </c>
@@ -6034,7 +6038,7 @@
         <v>0.10889857619531598</v>
       </c>
     </row>
-    <row r="124" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="30">
         <v>1979</v>
       </c>
@@ -6116,7 +6120,7 @@
         <v>0.50241347248615986</v>
       </c>
     </row>
-    <row r="126" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="30">
         <v>1981</v>
       </c>
@@ -6157,7 +6161,7 @@
         <v>0.59446812063878207</v>
       </c>
     </row>
-    <row r="127" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="30">
         <v>1982</v>
       </c>
@@ -6198,7 +6202,7 @@
         <v>0.57758597964130631</v>
       </c>
     </row>
-    <row r="128" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="30">
         <v>1983</v>
       </c>
@@ -6239,7 +6243,7 @@
         <v>0.28269596470231978</v>
       </c>
     </row>
-    <row r="129" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="30">
         <v>1984</v>
       </c>
@@ -6280,7 +6284,7 @@
         <v>0.43658570470016878</v>
       </c>
     </row>
-    <row r="130" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="30">
         <v>1985</v>
       </c>
@@ -6321,7 +6325,7 @@
         <v>0.44824142148510449</v>
       </c>
     </row>
-    <row r="131" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="30">
         <v>1986</v>
       </c>
@@ -6362,7 +6366,7 @@
         <v>0.59491114190432626</v>
       </c>
     </row>
-    <row r="132" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="30">
         <v>1987</v>
       </c>
@@ -6403,7 +6407,7 @@
         <v>0.66508130023348211</v>
       </c>
     </row>
-    <row r="133" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="30">
         <v>1988</v>
       </c>
@@ -6444,7 +6448,7 @@
         <v>0.80974002706645964</v>
       </c>
     </row>
-    <row r="134" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="30">
         <v>1989</v>
       </c>
@@ -6526,7 +6530,7 @@
         <v>1.1514043618001604</v>
       </c>
     </row>
-    <row r="136" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="30">
         <v>1991</v>
       </c>
@@ -6567,7 +6571,7 @@
         <v>1.2665031667018884</v>
       </c>
     </row>
-    <row r="137" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="30">
         <v>1992</v>
       </c>
@@ -6608,7 +6612,7 @@
         <v>0.95269925854566462</v>
       </c>
     </row>
-    <row r="138" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="30">
         <v>1993</v>
       </c>
@@ -6649,7 +6653,7 @@
         <v>0.8774082185490677</v>
       </c>
     </row>
-    <row r="139" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="30">
         <v>1994</v>
       </c>
@@ -6690,7 +6694,7 @@
         <v>0.72395053791523944</v>
       </c>
     </row>
-    <row r="140" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="30">
         <v>1995</v>
       </c>
@@ -6731,7 +6735,7 @@
         <v>0.61739396915722833</v>
       </c>
     </row>
-    <row r="141" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="30">
         <v>1996</v>
       </c>
@@ -6772,7 +6776,7 @@
         <v>0.26891883357871893</v>
       </c>
     </row>
-    <row r="142" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="30">
         <v>1997</v>
       </c>
@@ -6813,7 +6817,7 @@
         <v>0.21350460773982799</v>
       </c>
     </row>
-    <row r="143" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="30">
         <v>1998</v>
       </c>
@@ -6854,7 +6858,7 @@
         <v>0.38148571154793265</v>
       </c>
     </row>
-    <row r="144" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="30">
         <v>1999</v>
       </c>
@@ -6936,7 +6940,7 @@
         <v>0.55288309881408804</v>
       </c>
     </row>
-    <row r="146" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="20">
         <v>2001</v>
       </c>
@@ -6977,7 +6981,7 @@
         <v>0.80602831095423244</v>
       </c>
     </row>
-    <row r="147" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="20">
         <v>2002</v>
       </c>
@@ -7018,7 +7022,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="148" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="20">
         <v>2003</v>
       </c>
@@ -7059,7 +7063,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="149" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="20">
         <v>2004</v>
       </c>
@@ -7100,7 +7104,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="150" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="20">
         <v>2005</v>
       </c>
@@ -7141,7 +7145,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="151" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="20">
         <v>2006</v>
       </c>
@@ -7182,7 +7186,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="152" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="20">
         <v>2007</v>
       </c>
@@ -7223,7 +7227,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="153" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="20">
         <v>2008</v>
       </c>
@@ -7264,7 +7268,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="154" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="20">
         <v>2009</v>
       </c>
@@ -7346,7 +7350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="20">
         <v>2011</v>
       </c>
@@ -7387,7 +7391,7 @@
         <v>1.0740350799617897</v>
       </c>
     </row>
-    <row r="157" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="15">
         <v>2012</v>
       </c>
@@ -7428,7 +7432,7 @@
         <v>1.0609878836</v>
       </c>
     </row>
-    <row r="158" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="15">
         <v>2013</v>
       </c>
@@ -7469,7 +7473,7 @@
         <v>1.2510293492</v>
       </c>
     </row>
-    <row r="159" spans="1:13" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:13" s="34" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="15">
         <v>2014</v>
       </c>
@@ -7510,7 +7514,7 @@
         <v>1.2044157776</v>
       </c>
     </row>
-    <row r="160" spans="1:13" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:13" s="34" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="15">
         <v>2015</v>
       </c>
@@ -7551,7 +7555,7 @@
         <v>1.0859872202</v>
       </c>
     </row>
-    <row r="161" spans="1:13" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:13" s="34" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="15">
         <v>2016</v>
       </c>
@@ -7592,7 +7596,7 @@
         <v>1.1099147533</v>
       </c>
     </row>
-    <row r="162" spans="1:13" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:13" s="34" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="15">
         <v>2017</v>
       </c>
@@ -7633,7 +7637,7 @@
         <v>0.7670243659</v>
       </c>
     </row>
-    <row r="163" spans="1:13" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:13" s="34" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="15">
         <v>2018</v>
       </c>
@@ -7674,127 +7678,169 @@
         <v>0.7118820669</v>
       </c>
     </row>
-    <row r="164" spans="1:13" s="34" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A164" s="23">
+    <row r="164" spans="1:13" s="34" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A164" s="15">
         <v>2019</v>
       </c>
-      <c r="B164" s="35">
+      <c r="B164" s="33">
         <v>8544527</v>
       </c>
-      <c r="C164" s="35">
+      <c r="C164" s="33">
         <v>86172</v>
       </c>
-      <c r="D164" s="35">
+      <c r="D164" s="33">
         <v>67780</v>
       </c>
-      <c r="E164" s="35">
+      <c r="E164" s="33">
         <v>18392</v>
       </c>
-      <c r="F164" s="35">
+      <c r="F164" s="33">
         <v>169573</v>
       </c>
-      <c r="G164" s="35">
+      <c r="G164" s="33">
         <v>126221</v>
       </c>
-      <c r="H164" s="35">
+      <c r="H164" s="33">
         <v>43352</v>
       </c>
-      <c r="I164" s="35">
+      <c r="I164" s="33">
         <v>41127</v>
       </c>
-      <c r="J164" s="35">
+      <c r="J164" s="33">
         <v>-238</v>
       </c>
-      <c r="K164" s="35">
+      <c r="K164" s="33">
         <v>8606033</v>
       </c>
-      <c r="L164" s="35">
+      <c r="L164" s="33">
         <v>61506</v>
       </c>
-      <c r="M164" s="36">
+      <c r="M164" s="31">
         <v>0.71982919590000005</v>
       </c>
     </row>
-    <row r="165" spans="1:13" s="38" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A165" s="37" t="s">
+    <row r="165" spans="1:13" s="34" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A165" s="23">
+        <v>2020</v>
+      </c>
+      <c r="B165" s="35">
+        <v>8606033</v>
+      </c>
+      <c r="C165" s="35">
+        <v>85914</v>
+      </c>
+      <c r="D165" s="35">
+        <v>76195</v>
+      </c>
+      <c r="E165" s="35">
+        <v>9719</v>
+      </c>
+      <c r="F165" s="35">
+        <v>163180</v>
+      </c>
+      <c r="G165" s="35">
+        <v>109376</v>
+      </c>
+      <c r="H165" s="35">
+        <v>53804</v>
+      </c>
+      <c r="I165" s="35">
+        <v>34141</v>
+      </c>
+      <c r="J165" s="35">
+        <v>744</v>
+      </c>
+      <c r="K165" s="35">
+        <v>8670300</v>
+      </c>
+      <c r="L165" s="35">
+        <v>64267</v>
+      </c>
+      <c r="M165" s="36">
+        <v>0.74676683210000006</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" s="38" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A166" s="37" t="s">
         <v>16</v>
-      </c>
-      <c r="C165" s="39"/>
-      <c r="E165" s="14"/>
-      <c r="F165" s="14"/>
-    </row>
-    <row r="166" spans="1:13" s="38" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A166" s="14" t="s">
-        <v>8</v>
       </c>
       <c r="C166" s="39"/>
       <c r="E166" s="14"/>
       <c r="F166" s="14"/>
     </row>
-    <row r="167" spans="1:13" s="38" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A167" s="37" t="s">
+    <row r="167" spans="1:13" s="38" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A167" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C167" s="39"/>
+      <c r="E167" s="14"/>
+      <c r="F167" s="14"/>
+    </row>
+    <row r="168" spans="1:13" s="38" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A168" s="37" t="s">
         <v>19</v>
-      </c>
-      <c r="B167" s="30"/>
-      <c r="C167" s="39"/>
-    </row>
-    <row r="168" spans="1:13" s="38" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A168" s="37" t="s">
-        <v>23</v>
       </c>
       <c r="B168" s="30"/>
       <c r="C168" s="39"/>
     </row>
-    <row r="169" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:13" s="38" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B169" s="30"/>
+      <c r="C169" s="39"/>
+    </row>
+    <row r="170" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A170" s="37" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="170" spans="1:13" s="38" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A170" s="40" t="s">
+    <row r="171" spans="1:13" s="38" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A171" s="40" t="s">
         <v>28</v>
-      </c>
-      <c r="B170" s="30"/>
-      <c r="C170" s="39"/>
-    </row>
-    <row r="171" spans="1:13" s="38" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A171" s="41" t="s">
-        <v>11</v>
       </c>
       <c r="B171" s="30"/>
       <c r="C171" s="39"/>
     </row>
-    <row r="172" spans="1:13" s="38" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A172" s="37" t="s">
+    <row r="172" spans="1:13" s="38" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A172" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B172" s="30"/>
+      <c r="C172" s="39"/>
+    </row>
+    <row r="173" spans="1:13" s="38" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A173" s="37" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="173" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A173" s="37" t="s">
+    <row r="174" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A174" s="37" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="174" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A174" s="14" t="s">
+    <row r="175" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A175" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="175" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A175" s="14" t="s">
+    <row r="176" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A176" s="14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="176" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A176" s="14"/>
-    </row>
-    <row r="177" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A177" s="14" t="s">
+    <row r="177" spans="1:9" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A177" s="14"/>
+    </row>
+    <row r="178" spans="1:9" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A178" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I177" s="42"/>
-    </row>
-    <row r="179" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A179" s="14"/>
+      <c r="I178" s="42"/>
+    </row>
+    <row r="179" spans="1:9" ht="13.15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="180" spans="1:9" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A180" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>